<commit_message>
memperbarui data di file team_details
</commit_message>
<xml_diff>
--- a/team_details.xlsx
+++ b/team_details.xlsx
@@ -1,24 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\semester 7\Pembelajaran Mesin\versi 3\modul 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SEMESTER 7\PEMBELAJARAN MESIN\Tugas\ProjectML_261-235\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BDA8E5A-192E-406A-B0B3-10747FCC9AD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB1F27B-89BA-42F4-A25C-BA6B0835E448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{9C344D26-BD22-471F-826C-52DEB1F8CB82}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9C344D26-BD22-471F-826C-52DEB1F8CB82}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -42,29 +49,70 @@
     <t>Judul Artikel</t>
   </si>
   <si>
-    <t>1. Ulfah Nur Oktaviana</t>
-  </si>
-  <si>
     <t>2. Tiara Intana Sari</t>
   </si>
   <si>
-    <t>Penerapan Convolutional Neural Network pada Citra Rontgen Paru-Paru  untuk Deteksi SARS-CoV-2</t>
-  </si>
-  <si>
-    <t>Klasifikasi Covid-19 Menggunakan Citra X-Ray Radiology</t>
-  </si>
-  <si>
-    <t>https://www.kaggle.com/tawsifurrahman/covid19-radiography-database</t>
-  </si>
-  <si>
-    <t>http://jurnal.iaii.or.id/index.php/RESTI/article/view/3153</t>
+    <t xml:space="preserve">Klasifikasi Covid-19 Menggunakan Citra X-Ray Radiology
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Ulfah Nur Oktaviana
+</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">dataset 1:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>https://github.com/drkhan107/CoroNet</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+dataset 2:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>https://github.com/muhammedtalo/COVID-19</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Attention-based VGG-16 model for COVID-19 chest X-ray image
+classification
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://link.springer.com/article/10.1007/s10489-020-02055-x
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,6 +132,20 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="4"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -157,7 +219,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -169,6 +231,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
@@ -495,24 +560,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BA007E8-8263-42CB-9DF5-529D2D466376}">
-  <dimension ref="B2:F4"/>
+  <dimension ref="B2:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D3" sqref="B2:F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="1"/>
-    <col min="2" max="2" width="21.6328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="22.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.81640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.54296875" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="8.7109375" style="1"/>
+    <col min="2" max="2" width="21.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="29.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="27.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
@@ -529,31 +594,37 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B4" s="2" t="s">
-        <v>6</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="7"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="8"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E12" s="1">
+        <f ca="1">+E12:F26</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -563,10 +634,10 @@
     <mergeCell ref="F3:F4"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" xr:uid="{4D68B9D0-1CB2-49B3-9763-3D24479DA61A}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{ADBDE606-F435-4302-81EC-8AFD18F403ED}"/>
+    <hyperlink ref="E3:E4" r:id="rId1" display="https://link.springer.com/article/10.1007/s10489-020-02055-x" xr:uid="{4DCA5D83-F857-490C-8344-18D617A0AF8E}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{9B156C83-DFDE-47F9-8253-7268260B7988}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>